<commit_message>
added positive and negavtive test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/log.xlsx
+++ b/src/test/resources/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darshb\Desktop\MAIN_ASSIGNMENT_REST\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB1D35-37E3-442B-8E1A-908C202D3144}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E78D5-A998-46A4-9ADB-1E8BE5906FD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="1560" windowWidth="14400" windowHeight="7360" xr2:uid="{03A61A75-E8B8-4103-8A57-7A186AC969CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03A61A75-E8B8-4103-8A57-7A186AC969CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>sanj1@gmail.com</t>
+    <t>darsh3@gmail.com</t>
   </si>
   <si>
-    <t>harshi1@gmail.com</t>
+    <t>sanj3@gmail.com</t>
   </si>
   <si>
-    <t>darsh1@gmail.com</t>
+    <t>harshi3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9A3277-281D-4A49-B3B0-6718650F52A4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -417,7 +419,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>12345678</v>
@@ -425,7 +427,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>12345678</v>
@@ -433,7 +435,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>12345678</v>

</xml_diff>